<commit_message>
Update email template and sending logic
Enhanced the HTML email template with improved styling, images, and QR code for Telegram bot installation. Changed sender email, subject line, and increased delay between emails. Improved mail transporter configuration for better compatibility.
</commit_message>
<xml_diff>
--- a/emails.xlsx
+++ b/emails.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\React\Mailer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C257C45-B2C5-4B25-A715-E8DAE9186259}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3816898A-9F10-4717-B35F-FF9153BE8E60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,16 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
-  <si>
-    <t>d.kovbasiuk@grmu.com.ua</t>
-  </si>
-  <si>
-    <t>m.tasalova@grmu.com.ua</t>
-  </si>
-  <si>
-    <t>o.reznik@grmu.com.ua</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>email</t>
   </si>
@@ -379,45 +370,39 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
     </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1"/>
+    </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>2</v>
-      </c>
+      <c r="A4" s="1"/>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>4</v>
-      </c>
+      <c r="A5" s="1"/>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A4" r:id="rId1" xr:uid="{7E134908-3D13-45DF-91E1-15C555BB49CA}"/>
-    <hyperlink ref="A3" r:id="rId2" xr:uid="{41F98953-5DAE-45BB-959A-B7E9E5F6A7C9}"/>
-    <hyperlink ref="A2" r:id="rId3" xr:uid="{66CC1BBB-E49A-4B5C-858B-B4AFE016FC19}"/>
-    <hyperlink ref="A5" r:id="rId4" xr:uid="{AE132074-48E2-4769-A6D1-BE90385E571A}"/>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{0560F80F-F3E2-4066-BF62-02D37BC9148F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>